<commit_message>
amélioration de la multithreadisation
</commit_message>
<xml_diff>
--- a/resultats.xlsx
+++ b/resultats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrien/Documents/Informatique/Python/td_taxidriver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCD19B9-6C14-F74E-9F36-96B3ABB6AE96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C59088B-B623-944E-ACE7-2A01283598F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="1300" windowWidth="28040" windowHeight="17040" xr2:uid="{5558E801-2638-2347-BC94-56BADB05DCFF}"/>
+    <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{5558E801-2638-2347-BC94-56BADB05DCFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FBD1BA-B0B2-7C46-8220-393BD424CC73}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Mise à jour du fichier excel
</commit_message>
<xml_diff>
--- a/resultats.xlsx
+++ b/resultats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrien/Documents/Informatique/Python/td_taxidriver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C59088B-B623-944E-ACE7-2A01283598F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13220110-8B03-9F4E-8278-DE99B81A821B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{5558E801-2638-2347-BC94-56BADB05DCFF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Random Forest Regressor</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>le temps d'exécution est mesuré en secondes sur processeur intel core i5 - 6500</t>
+  </si>
+  <si>
+    <t>plusieurs fit chacun sur un thread</t>
+  </si>
+  <si>
+    <t>truc normal</t>
+  </si>
+  <si>
+    <t>fit() sur 3 threads</t>
+  </si>
+  <si>
+    <t>fit() sur 4 threads</t>
   </si>
 </sst>
 </file>
@@ -85,12 +97,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,9 +135,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,15 +457,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FBD1BA-B0B2-7C46-8220-393BD424CC73}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -438,17 +473,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -458,8 +493,9 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -479,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10</v>
       </c>
@@ -499,7 +535,7 @@
         <v>500.76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>10</v>
       </c>
@@ -516,7 +552,7 @@
         <v>428.92</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10</v>
       </c>
@@ -533,7 +569,7 @@
         <v>411.04</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -550,7 +586,7 @@
         <v>416.63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -567,7 +603,7 @@
         <v>418.19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -584,24 +620,36 @@
         <v>415.01</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13">
         <v>70</v>
       </c>
+      <c r="C13">
+        <v>240</v>
+      </c>
+      <c r="D13">
+        <v>374.31</v>
+      </c>
       <c r="F13">
         <v>415.96</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14">
         <v>80</v>
       </c>
+      <c r="C14">
+        <v>240</v>
+      </c>
+      <c r="D14">
+        <v>372.24</v>
+      </c>
       <c r="E14">
         <v>142</v>
       </c>
@@ -609,13 +657,19 @@
         <v>415.97</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>10</v>
       </c>
       <c r="B15">
         <v>90</v>
       </c>
+      <c r="C15">
+        <v>243</v>
+      </c>
+      <c r="D15">
+        <v>372.24</v>
+      </c>
       <c r="E15">
         <v>141</v>
       </c>
@@ -623,13 +677,19 @@
         <v>415.97</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>
       <c r="B16">
         <v>100</v>
       </c>
+      <c r="C16">
+        <v>237</v>
+      </c>
+      <c r="D16">
+        <v>372.24</v>
+      </c>
       <c r="E16">
         <v>142</v>
       </c>
@@ -637,7 +697,7 @@
         <v>415.97</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20</v>
       </c>
@@ -654,24 +714,24 @@
         <v>502.49</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20</v>
       </c>
       <c r="B18">
         <v>20</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>247</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>400.44</v>
       </c>
       <c r="F18">
         <v>425.3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20</v>
       </c>
@@ -688,7 +748,7 @@
         <v>406.61</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20</v>
       </c>
@@ -705,7 +765,7 @@
         <v>409.3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -722,7 +782,7 @@
         <v>408.76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -739,26 +799,36 @@
         <v>406.36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
       <c r="B23">
         <v>70</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="C23" s="4">
+        <v>473</v>
+      </c>
+      <c r="D23" s="5">
+        <v>374.55</v>
+      </c>
       <c r="F23">
         <v>409.24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="B24">
         <v>80</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="C24" s="4">
+        <v>476</v>
+      </c>
+      <c r="D24" s="5">
+        <v>373.48</v>
+      </c>
       <c r="E24">
         <v>252</v>
       </c>
@@ -766,14 +836,19 @@
         <v>409.24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20</v>
       </c>
       <c r="B25">
         <v>90</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="C25" s="4">
+        <v>471</v>
+      </c>
+      <c r="D25" s="5">
+        <v>373.48</v>
+      </c>
       <c r="E25">
         <v>278</v>
       </c>
@@ -781,14 +856,19 @@
         <v>409.24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26">
         <v>100</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="C26" s="4">
+        <v>469</v>
+      </c>
+      <c r="D26" s="5">
+        <v>373.48</v>
+      </c>
       <c r="E26">
         <v>279</v>
       </c>
@@ -796,7 +876,7 @@
         <v>409.24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>30</v>
       </c>
@@ -813,7 +893,7 @@
         <v>500.48</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>30</v>
       </c>
@@ -830,7 +910,7 @@
         <v>417.51</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>30</v>
       </c>
@@ -847,7 +927,7 @@
         <v>395.44</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>30</v>
       </c>
@@ -863,8 +943,11 @@
       <c r="F30">
         <v>396.72</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -880,8 +963,11 @@
       <c r="F31">
         <v>397.01</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I31" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -897,25 +983,43 @@
       <c r="F32">
         <v>395.69</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I32" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
       <c r="B33">
         <v>70</v>
       </c>
+      <c r="C33" s="4">
+        <v>703</v>
+      </c>
+      <c r="D33" s="4">
+        <v>368.23</v>
+      </c>
       <c r="F33">
         <v>394.75</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I33" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>30</v>
       </c>
       <c r="B34">
         <v>80</v>
       </c>
+      <c r="C34" s="4">
+        <v>700</v>
+      </c>
+      <c r="D34" s="4">
+        <v>367.52</v>
+      </c>
       <c r="E34">
         <v>425</v>
       </c>
@@ -923,13 +1027,19 @@
         <v>394.75</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>30</v>
       </c>
       <c r="B35">
         <v>90</v>
       </c>
+      <c r="C35" s="4">
+        <v>688</v>
+      </c>
+      <c r="D35" s="4">
+        <v>367.52</v>
+      </c>
       <c r="E35">
         <v>410</v>
       </c>
@@ -937,114 +1047,312 @@
         <v>394.75</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
       <c r="B36">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="4">
+        <v>672</v>
+      </c>
+      <c r="D36" s="4">
+        <v>367.52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>40</v>
       </c>
       <c r="B37">
         <v>40</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>729</v>
       </c>
       <c r="D37">
         <v>361.43</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>40</v>
       </c>
       <c r="B38">
         <v>50</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <v>765</v>
       </c>
       <c r="D38">
         <v>362.64</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>40</v>
       </c>
       <c r="B39">
         <v>60</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="2">
         <v>720</v>
       </c>
       <c r="D39">
         <v>362.71</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>50</v>
       </c>
       <c r="B40">
         <v>40</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>912</v>
       </c>
       <c r="D40">
         <v>359.21</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>50</v>
       </c>
       <c r="B41">
         <v>50</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>929</v>
       </c>
       <c r="D41">
         <v>359.5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>50</v>
       </c>
       <c r="B42">
         <v>60</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C42" s="3">
+        <v>394</v>
+      </c>
+      <c r="D42" s="3">
+        <v>359.47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>60</v>
       </c>
       <c r="B43">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C43" s="3">
+        <v>468</v>
+      </c>
+      <c r="D43" s="3">
+        <v>356.29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>60</v>
       </c>
       <c r="B44">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C44" s="3">
+        <v>465</v>
+      </c>
+      <c r="D44" s="3">
+        <v>356.31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>60</v>
       </c>
       <c r="B45">
         <v>60</v>
+      </c>
+      <c r="C45" s="3">
+        <v>466</v>
+      </c>
+      <c r="D45" s="3">
+        <v>356.21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>70</v>
+      </c>
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46" s="6">
+        <v>419</v>
+      </c>
+      <c r="D46" s="6">
+        <v>358.67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>70</v>
+      </c>
+      <c r="B47">
+        <v>40</v>
+      </c>
+      <c r="C47" s="6">
+        <v>454</v>
+      </c>
+      <c r="D47" s="6">
+        <v>355.18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>70</v>
+      </c>
+      <c r="B48">
+        <v>50</v>
+      </c>
+      <c r="C48" s="6">
+        <v>465</v>
+      </c>
+      <c r="D48" s="6">
+        <v>354.94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>80</v>
+      </c>
+      <c r="B49">
+        <v>30</v>
+      </c>
+      <c r="C49" s="6">
+        <v>478</v>
+      </c>
+      <c r="D49" s="6">
+        <v>358.17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>80</v>
+      </c>
+      <c r="B50">
+        <v>40</v>
+      </c>
+      <c r="C50" s="6">
+        <v>520</v>
+      </c>
+      <c r="D50" s="6">
+        <v>354.48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>80</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51" s="6">
+        <v>524</v>
+      </c>
+      <c r="D51" s="6">
+        <v>354.6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>90</v>
+      </c>
+      <c r="B52">
+        <v>30</v>
+      </c>
+      <c r="C52" s="6">
+        <v>533</v>
+      </c>
+      <c r="D52" s="6">
+        <v>354.64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>90</v>
+      </c>
+      <c r="B53">
+        <v>40</v>
+      </c>
+      <c r="C53" s="6">
+        <v>580</v>
+      </c>
+      <c r="D53" s="6">
+        <v>350.78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>90</v>
+      </c>
+      <c r="B54">
+        <v>50</v>
+      </c>
+      <c r="C54" s="6">
+        <v>595</v>
+      </c>
+      <c r="D54" s="6">
+        <v>350.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>100</v>
+      </c>
+      <c r="B55">
+        <v>30</v>
+      </c>
+      <c r="C55" s="6">
+        <v>593</v>
+      </c>
+      <c r="D55" s="6">
+        <v>354.76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>100</v>
+      </c>
+      <c r="B56">
+        <v>40</v>
+      </c>
+      <c r="C56" s="6">
+        <v>644</v>
+      </c>
+      <c r="D56" s="6">
+        <v>351.47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>100</v>
+      </c>
+      <c r="B57">
+        <v>50</v>
+      </c>
+      <c r="C57" s="6">
+        <v>659</v>
+      </c>
+      <c r="D57" s="6">
+        <v>351.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>